<commit_message>
migrate read to use multiple devices
</commit_message>
<xml_diff>
--- a/hardware/eagle/bbb-cc2520/rev_a/bbb-cc2520_a_bom.xlsx
+++ b/hardware/eagle/bbb-cc2520/rev_a/bbb-cc2520_a_bom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="192">
   <si>
     <t>Qty</t>
   </si>
@@ -1452,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2195,9 +2195,7 @@
       <c r="I25" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>168</v>
-      </c>
+      <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>